<commit_message>
add nipah virus result
</commit_message>
<xml_diff>
--- a/OutputData/Nipah/Nipah_Combined_12_11.xlsx
+++ b/OutputData/Nipah/Nipah_Combined_12_11.xlsx
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>authors</t>
+          <t>Authors</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>journal</t>
+          <t>Journal</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>pmid</t>
+          <t>PMID</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">

</xml_diff>